<commit_message>
Registro de Cambios a Requerimientos
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_REQM/RCREQM/RCREQM_V1.1_2015.xlsx
+++ b/Area_de_Proceso-_REQM/RCREQM/RCREQM_V1.1_2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thefa\Downloads\UTP-GPS-ALARM-master\Area_de_Proceso-_REQM\RCREQM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTP-GPS-ALARM\UTP-GPS-ALARM\Area_de_Proceso-_REQM\RCREQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="Situación">#REF!</definedName>
     <definedName name="TARIFA_VIGENTE">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,9 +74,6 @@
     <t>RCREQM Registro de Cambios de Requerimientos</t>
   </si>
   <si>
-    <t>Versión: 1.0</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Responsable de tomar la decisión</t>
   </si>
   <si>
-    <t>REGISTRO DE CAMBIOS DE REQUERIMIENTOS DEL PROYECTO</t>
-  </si>
-  <si>
     <t>Aprobado</t>
   </si>
   <si>
@@ -225,16 +219,22 @@
   </si>
   <si>
     <t>UTP-GPS-ALARM</t>
+  </si>
+  <si>
+    <t>RCREQM REGISTRO DE CAMBIOS DE REQUERIMIENTOS DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>Versión: 1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +362,13 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -482,7 +489,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -517,10 +524,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -714,9 +717,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -725,32 +725,89 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -762,96 +819,47 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1445,157 +1453,150 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="18" style="16" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="3" width="9.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="18" style="15" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="86" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="15"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="24">
-      <c r="A4" s="15"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="85">
+      <c r="A5" s="14"/>
+      <c r="B5" s="84">
         <v>1</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="86">
+        <v>42290</v>
+      </c>
+      <c r="E5" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="88">
-        <v>42290</v>
-      </c>
-      <c r="E5" s="85" t="s">
+      <c r="F5" s="84" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="84" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="14"/>
+      <c r="B7" s="84">
+        <v>1</v>
+      </c>
+      <c r="C7" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="85" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="85" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="15"/>
-      <c r="B7" s="85">
-        <v>1</v>
-      </c>
-      <c r="C7" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="88">
+      <c r="D7" s="86">
         <v>42313</v>
       </c>
-      <c r="E7" s="85" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="85" t="s">
+      <c r="E7" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="85" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="15"/>
+      <c r="H7" s="84" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="B8" s="85"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="10" spans="1:9" ht="48" customHeight="1"/>
     <row r="11" spans="1:9" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="B2:H2"/>
@@ -1604,6 +1605,13 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1613,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I184"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:C23"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1629,205 +1637,205 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="48.75" customHeight="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="116" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="118"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="92"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="18"/>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="95"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.5">
+      <c r="A5" s="17"/>
+      <c r="B5" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:8" ht="17.25" customHeight="1">
+      <c r="A6" s="17"/>
+      <c r="B6" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
+    </row>
+    <row r="7" spans="1:8" s="28" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="17"/>
+      <c r="B9" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="119" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="121"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:8" ht="13.5">
-      <c r="A5" s="18"/>
-      <c r="B5" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="122" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
-    </row>
-    <row r="7" spans="1:8" s="29" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="18"/>
-      <c r="B9" s="125" t="s">
+      <c r="C9" s="99"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="99" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="99"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="17"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:8" ht="12" customHeight="1">
+      <c r="A11" s="17"/>
+      <c r="B11" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="125"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="125" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="125"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="18"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:8" ht="12" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="126" t="s">
+      <c r="C11" s="88"/>
+      <c r="E11" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="126"/>
-      <c r="E11" s="113" t="s">
+      <c r="F11" s="89"/>
+    </row>
+    <row r="12" spans="1:8" ht="9.9499999999999993" customHeight="1">
+      <c r="A12" s="17"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+    </row>
+    <row r="13" spans="1:8" ht="12" customHeight="1">
+      <c r="A13" s="17"/>
+      <c r="B13" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="103"/>
+      <c r="E13" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="113"/>
-    </row>
-    <row r="12" spans="1:8" ht="9.9499999999999993" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-    </row>
-    <row r="13" spans="1:8" ht="12" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="112" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="112"/>
-      <c r="E13" s="113" t="s">
+      <c r="F13" s="89"/>
+    </row>
+    <row r="14" spans="1:8" ht="9.9499999999999993" customHeight="1">
+      <c r="A14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="12" customHeight="1">
+      <c r="A15" s="32"/>
+      <c r="B15" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="104"/>
+      <c r="E15" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="113"/>
-    </row>
-    <row r="14" spans="1:8" ht="9.9499999999999993" customHeight="1">
-      <c r="A14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" ht="12" customHeight="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="114" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="114"/>
-      <c r="E15" s="113" t="s">
+      <c r="F15" s="89"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="32"/>
+    </row>
+    <row r="17" spans="1:9" ht="12" customHeight="1">
+      <c r="A17" s="32"/>
+      <c r="B17" s="105" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="105"/>
+      <c r="E17" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="113"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" ht="12" customHeight="1">
-      <c r="A17" s="33"/>
-      <c r="B17" s="115" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="115"/>
-      <c r="E17" s="113" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="113"/>
-      <c r="I17" s="34"/>
+      <c r="F17" s="89"/>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A18" s="35"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="I18" s="36"/>
+      <c r="I18" s="35"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="33"/>
-    </row>
-    <row r="20" spans="1:9" s="37" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B20" s="108" t="s">
+      <c r="A19" s="32"/>
+    </row>
+    <row r="20" spans="1:9" s="36" customFormat="1" ht="16.5" customHeight="1">
+      <c r="B20" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+    </row>
+    <row r="21" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B21" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="108"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="108"/>
-    </row>
-    <row r="21" spans="1:9" s="37" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B21" s="109" t="s">
+      <c r="C21" s="108"/>
+      <c r="D21" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+    </row>
+    <row r="22" spans="1:9" s="36" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B22" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="110"/>
-      <c r="D21" s="111" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
-    </row>
-    <row r="22" spans="1:9" s="37" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B22" s="104" t="s">
+      <c r="C22" s="101"/>
+      <c r="D22" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="103" t="s">
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+    </row>
+    <row r="23" spans="1:9" s="36" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B23" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
-    </row>
-    <row r="23" spans="1:9" s="37" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B23" s="104" t="s">
+      <c r="C23" s="101"/>
+      <c r="D23" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="103" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-    </row>
-    <row r="24" spans="1:9" s="37" customFormat="1" ht="13.5" customHeight="1">
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+    </row>
+    <row r="24" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -1835,196 +1843,196 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:9" ht="13.5">
-      <c r="A25" s="33"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:9" s="37" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B26" s="108" t="s">
+    <row r="26" spans="1:9" s="36" customFormat="1" ht="16.5" customHeight="1">
+      <c r="B26" s="106" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+    </row>
+    <row r="27" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B27" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="108"/>
+      <c r="D27" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+    </row>
+    <row r="28" spans="1:9" s="36" customFormat="1">
+      <c r="B28" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="108"/>
-      <c r="D26" s="108"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="108"/>
-    </row>
-    <row r="27" spans="1:9" s="37" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B27" s="109" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="110"/>
-      <c r="D27" s="111" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-    </row>
-    <row r="28" spans="1:9" s="37" customFormat="1">
-      <c r="B28" s="106" t="s">
+      <c r="C28" s="112"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+    </row>
+    <row r="29" spans="1:9" s="36" customFormat="1">
+      <c r="B29" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="106"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-    </row>
-    <row r="29" spans="1:9" s="37" customFormat="1">
-      <c r="B29" s="101" t="s">
+      <c r="C29" s="111"/>
+      <c r="D29" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="102"/>
-      <c r="D29" s="103" t="s">
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="32"/>
+      <c r="B30" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="103"/>
-      <c r="F29" s="103"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="33"/>
-      <c r="B30" s="106" t="s">
+      <c r="C30" s="112"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="113"/>
+      <c r="F30" s="113"/>
+    </row>
+    <row r="31" spans="1:9" s="38" customFormat="1">
+      <c r="A31" s="37"/>
+      <c r="B31" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="106"/>
-      <c r="D30" s="107"/>
-      <c r="E30" s="107"/>
-      <c r="F30" s="107"/>
-    </row>
-    <row r="31" spans="1:9" s="39" customFormat="1">
-      <c r="A31" s="38"/>
-      <c r="B31" s="101" t="s">
+      <c r="C31" s="111"/>
+      <c r="D31" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="102"/>
-      <c r="D31" s="103" t="s">
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
+    </row>
+    <row r="32" spans="1:9" s="38" customFormat="1">
+      <c r="A32" s="37"/>
+      <c r="B32" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-    </row>
-    <row r="32" spans="1:9" s="39" customFormat="1">
-      <c r="A32" s="38"/>
-      <c r="B32" s="101" t="s">
+      <c r="C32" s="111"/>
+      <c r="D32" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="102"/>
-      <c r="D32" s="103" t="s">
+      <c r="E32" s="102"/>
+      <c r="F32" s="102"/>
+    </row>
+    <row r="33" spans="1:9" s="38" customFormat="1">
+      <c r="A33" s="37"/>
+      <c r="B33" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103"/>
-    </row>
-    <row r="33" spans="1:9" s="39" customFormat="1">
-      <c r="A33" s="38"/>
-      <c r="B33" s="101" t="s">
+      <c r="C33" s="111"/>
+      <c r="D33" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="102"/>
+      <c r="F33" s="102"/>
+    </row>
+    <row r="34" spans="1:9" s="38" customFormat="1">
+      <c r="A34" s="37"/>
+      <c r="B34" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="102"/>
-      <c r="D33" s="103" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="103"/>
-      <c r="F33" s="103"/>
-    </row>
-    <row r="34" spans="1:9" s="39" customFormat="1">
-      <c r="A34" s="38"/>
-      <c r="B34" s="101" t="s">
+      <c r="C34" s="111"/>
+      <c r="D34" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="102"/>
-      <c r="D34" s="103" t="s">
+      <c r="E34" s="102"/>
+      <c r="F34" s="102"/>
+    </row>
+    <row r="35" spans="1:9" s="38" customFormat="1">
+      <c r="A35" s="37"/>
+      <c r="B35" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
-    </row>
-    <row r="35" spans="1:9" s="39" customFormat="1">
-      <c r="A35" s="38"/>
-      <c r="B35" s="101" t="s">
+      <c r="C35" s="111"/>
+      <c r="D35" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="102"/>
-      <c r="D35" s="103" t="s">
+      <c r="E35" s="102"/>
+      <c r="F35" s="102"/>
+    </row>
+    <row r="36" spans="1:9" s="38" customFormat="1">
+      <c r="A36" s="37"/>
+      <c r="B36" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-    </row>
-    <row r="36" spans="1:9" s="39" customFormat="1">
-      <c r="A36" s="38"/>
-      <c r="B36" s="101" t="s">
+      <c r="C36" s="111"/>
+      <c r="D36" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="102"/>
-      <c r="D36" s="103" t="s">
+      <c r="E36" s="102"/>
+      <c r="F36" s="102"/>
+    </row>
+    <row r="37" spans="1:9" s="38" customFormat="1">
+      <c r="A37" s="37"/>
+      <c r="B37" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="103"/>
-      <c r="F36" s="103"/>
-    </row>
-    <row r="37" spans="1:9" s="39" customFormat="1">
-      <c r="A37" s="38"/>
-      <c r="B37" s="101" t="s">
+      <c r="C37" s="111"/>
+      <c r="D37" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="102"/>
-      <c r="D37" s="103" t="s">
+      <c r="E37" s="102"/>
+      <c r="F37" s="102"/>
+    </row>
+    <row r="38" spans="1:9" s="38" customFormat="1">
+      <c r="A38" s="37"/>
+      <c r="B38" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="103"/>
-      <c r="F37" s="103"/>
-    </row>
-    <row r="38" spans="1:9" s="39" customFormat="1">
-      <c r="A38" s="38"/>
-      <c r="B38" s="104" t="s">
+      <c r="C38" s="101"/>
+      <c r="D38" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="105"/>
-      <c r="D38" s="103" t="s">
+      <c r="E38" s="102"/>
+      <c r="F38" s="102"/>
+    </row>
+    <row r="39" spans="1:9" s="38" customFormat="1">
+      <c r="A39" s="37"/>
+      <c r="B39" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
-    </row>
-    <row r="39" spans="1:9" s="39" customFormat="1">
-      <c r="A39" s="38"/>
-      <c r="B39" s="104" t="s">
+      <c r="C39" s="101"/>
+      <c r="D39" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="105"/>
-      <c r="D39" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="103"/>
-      <c r="F39" s="103"/>
+      <c r="E39" s="102"/>
+      <c r="F39" s="102"/>
     </row>
     <row r="40" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A40" s="33"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
     </row>
     <row r="41" spans="1:9" ht="13.5">
-      <c r="A41" s="33"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:9" hidden="1">
-      <c r="A42" s="33"/>
-      <c r="B42" s="98" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="98"/>
-      <c r="D42" s="99"/>
-      <c r="E42" s="99"/>
-      <c r="F42" s="99"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="115"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="116"/>
+      <c r="F42" s="116"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" hidden="1" customHeight="1">
-      <c r="A43" s="33"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="8" t="s">
         <v>2</v>
       </c>
@@ -2036,897 +2044,897 @@
         <v>4</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
+        <v>53</v>
+      </c>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
     </row>
     <row r="44" spans="1:9" hidden="1">
-      <c r="A44" s="33"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
     </row>
     <row r="45" spans="1:9" hidden="1">
-      <c r="A45" s="33"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" hidden="1" customHeight="1">
-      <c r="A46" s="33"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" hidden="1" customHeight="1">
-      <c r="A47" s="33"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" hidden="1" customHeight="1">
-      <c r="A48" s="33"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="41"/>
     </row>
     <row r="49" spans="1:9" hidden="1">
-      <c r="A49" s="35"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="35"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="100"/>
-      <c r="D50" s="100"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="117"/>
+      <c r="C50" s="117"/>
+      <c r="D50" s="117"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="35"/>
-      <c r="B51" s="100"/>
-      <c r="C51" s="100"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="117"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="35"/>
-      <c r="B52" s="52"/>
-      <c r="C52" s="52"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="53"/>
+      <c r="E52" s="52"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="42"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="35"/>
-      <c r="B53" s="52"/>
-      <c r="C53" s="52"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="53"/>
+      <c r="E53" s="52"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="42"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="35"/>
-      <c r="B54" s="52"/>
-      <c r="C54" s="52"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="53"/>
+      <c r="E54" s="52"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="42"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="41"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="35"/>
-      <c r="B55" s="52"/>
-      <c r="C55" s="52"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="51"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="53"/>
+      <c r="E55" s="52"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="42"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="41"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="35"/>
-      <c r="B56" s="52"/>
-      <c r="C56" s="52"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="51"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="53"/>
+      <c r="E56" s="52"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="42"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
     </row>
     <row r="57" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A57" s="35"/>
-      <c r="B57" s="52"/>
-      <c r="C57" s="52"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="42"/>
+      <c r="G57" s="41"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="41"/>
     </row>
     <row r="58" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A58" s="35"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="96"/>
-      <c r="D58" s="96"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="114"/>
+      <c r="C58" s="114"/>
+      <c r="D58" s="114"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="41"/>
     </row>
     <row r="59" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A59" s="35"/>
-      <c r="B59" s="52"/>
-      <c r="C59" s="52"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="42"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+      <c r="I59" s="41"/>
     </row>
     <row r="60" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A60" s="35"/>
-      <c r="B60" s="52"/>
-      <c r="C60" s="52"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="51"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="42"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+      <c r="I60" s="41"/>
     </row>
     <row r="61" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A61" s="35"/>
-      <c r="B61" s="96"/>
-      <c r="C61" s="96"/>
-      <c r="D61" s="96"/>
-      <c r="E61" s="54"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="114"/>
+      <c r="C61" s="114"/>
+      <c r="D61" s="114"/>
+      <c r="E61" s="53"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="42"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="41"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="35"/>
-      <c r="B62" s="52"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="42"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+      <c r="I62" s="41"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="35"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="51"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="42"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="41"/>
+      <c r="I63" s="41"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="35"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="52"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="51"/>
+      <c r="C64" s="51"/>
+      <c r="D64" s="51"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="42"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="41"/>
+      <c r="I64" s="41"/>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="35"/>
-      <c r="B65" s="52"/>
-      <c r="C65" s="52"/>
-      <c r="D65" s="52"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="42"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+      <c r="I65" s="41"/>
     </row>
     <row r="66" spans="1:9" ht="27.75" customHeight="1">
-      <c r="A66" s="35"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="96"/>
-      <c r="E66" s="54"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="114"/>
+      <c r="D66" s="114"/>
+      <c r="E66" s="53"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="42"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="35"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="52"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="42"/>
+      <c r="G67" s="41"/>
+      <c r="H67" s="41"/>
+      <c r="I67" s="41"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="35"/>
-      <c r="B68" s="52"/>
-      <c r="C68" s="52"/>
-      <c r="D68" s="52"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="42"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="42"/>
+      <c r="G68" s="41"/>
+      <c r="H68" s="41"/>
+      <c r="I68" s="41"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="35"/>
-      <c r="B69" s="55"/>
-      <c r="C69" s="55"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="54"/>
+      <c r="C69" s="54"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="42"/>
-      <c r="H69" s="42"/>
-      <c r="I69" s="42"/>
+      <c r="G69" s="41"/>
+      <c r="H69" s="41"/>
+      <c r="I69" s="41"/>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1">
-      <c r="A70" s="35"/>
-      <c r="B70" s="55"/>
-      <c r="C70" s="55"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="56"/>
-      <c r="I70" s="56"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="54"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="55"/>
+      <c r="I70" s="55"/>
     </row>
     <row r="71" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A71" s="35"/>
-      <c r="B71" s="57"/>
-      <c r="C71" s="57"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="56"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="42"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="42"/>
+      <c r="G71" s="41"/>
+      <c r="H71" s="41"/>
+      <c r="I71" s="41"/>
     </row>
     <row r="72" spans="1:9" ht="13.5">
-      <c r="A72" s="35"/>
-      <c r="B72" s="57"/>
-      <c r="C72" s="57"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="56"/>
+      <c r="C72" s="56"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="42"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="42"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="41"/>
+      <c r="I72" s="41"/>
     </row>
     <row r="73" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A73" s="35"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="96"/>
-      <c r="D73" s="96"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="114"/>
+      <c r="C73" s="114"/>
+      <c r="D73" s="114"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="42"/>
-      <c r="H73" s="42"/>
-      <c r="I73" s="42"/>
+      <c r="G73" s="41"/>
+      <c r="H73" s="41"/>
+      <c r="I73" s="41"/>
     </row>
     <row r="74" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A74" s="35"/>
-      <c r="B74" s="96"/>
-      <c r="C74" s="96"/>
-      <c r="D74" s="96"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="114"/>
+      <c r="C74" s="114"/>
+      <c r="D74" s="114"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="42"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="42"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="41"/>
+      <c r="I74" s="41"/>
     </row>
     <row r="75" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A75" s="35"/>
-      <c r="B75" s="96"/>
-      <c r="C75" s="96"/>
-      <c r="D75" s="96"/>
+      <c r="A75" s="34"/>
+      <c r="B75" s="114"/>
+      <c r="C75" s="114"/>
+      <c r="D75" s="114"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="42"/>
-      <c r="H75" s="42"/>
-      <c r="I75" s="42"/>
+      <c r="G75" s="41"/>
+      <c r="H75" s="41"/>
+      <c r="I75" s="41"/>
     </row>
     <row r="76" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A76" s="35"/>
-      <c r="B76" s="96"/>
-      <c r="C76" s="96"/>
-      <c r="D76" s="96"/>
-      <c r="E76" s="54"/>
+      <c r="A76" s="34"/>
+      <c r="B76" s="114"/>
+      <c r="C76" s="114"/>
+      <c r="D76" s="114"/>
+      <c r="E76" s="53"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="42"/>
-      <c r="H76" s="42"/>
-      <c r="I76" s="42"/>
+      <c r="G76" s="41"/>
+      <c r="H76" s="41"/>
+      <c r="I76" s="41"/>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="35"/>
-      <c r="B77" s="58"/>
-      <c r="C77" s="58"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="57"/>
+      <c r="C77" s="57"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="42"/>
-      <c r="H77" s="42"/>
-      <c r="I77" s="42"/>
+      <c r="G77" s="41"/>
+      <c r="H77" s="41"/>
+      <c r="I77" s="41"/>
     </row>
     <row r="78" spans="1:9" ht="13.5">
-      <c r="A78" s="35"/>
-      <c r="B78" s="57"/>
-      <c r="C78" s="57"/>
+      <c r="A78" s="34"/>
+      <c r="B78" s="56"/>
+      <c r="C78" s="56"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="42"/>
-      <c r="H78" s="42"/>
-      <c r="I78" s="42"/>
+      <c r="G78" s="41"/>
+      <c r="H78" s="41"/>
+      <c r="I78" s="41"/>
     </row>
     <row r="79" spans="1:9" ht="13.5">
-      <c r="A79" s="35"/>
-      <c r="B79" s="57"/>
-      <c r="C79" s="57"/>
+      <c r="A79" s="34"/>
+      <c r="B79" s="56"/>
+      <c r="C79" s="56"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="42"/>
-      <c r="I79" s="42"/>
+      <c r="G79" s="41"/>
+      <c r="H79" s="41"/>
+      <c r="I79" s="41"/>
     </row>
     <row r="80" spans="1:9" ht="13.5">
-      <c r="A80" s="35"/>
-      <c r="B80" s="59"/>
-      <c r="C80" s="59"/>
+      <c r="A80" s="34"/>
+      <c r="B80" s="58"/>
+      <c r="C80" s="58"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="42"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="42"/>
+      <c r="G80" s="41"/>
+      <c r="H80" s="41"/>
+      <c r="I80" s="41"/>
     </row>
     <row r="81" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A81" s="33"/>
-      <c r="B81" s="60"/>
-      <c r="C81" s="60"/>
-      <c r="F81" s="61"/>
-      <c r="G81" s="42"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="42"/>
+      <c r="A81" s="32"/>
+      <c r="B81" s="59"/>
+      <c r="C81" s="59"/>
+      <c r="F81" s="60"/>
+      <c r="G81" s="41"/>
+      <c r="H81" s="41"/>
+      <c r="I81" s="41"/>
     </row>
     <row r="82" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A82" s="35"/>
-      <c r="B82" s="57"/>
-      <c r="C82" s="57"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="56"/>
+      <c r="C82" s="56"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="42"/>
-      <c r="H82" s="42"/>
-      <c r="I82" s="42"/>
+      <c r="G82" s="41"/>
+      <c r="H82" s="41"/>
+      <c r="I82" s="41"/>
     </row>
     <row r="83" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A83" s="35"/>
-      <c r="B83" s="59"/>
-      <c r="C83" s="59"/>
+      <c r="A83" s="34"/>
+      <c r="B83" s="58"/>
+      <c r="C83" s="58"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
-      <c r="G83" s="42"/>
-      <c r="H83" s="42"/>
-      <c r="I83" s="42"/>
+      <c r="G83" s="41"/>
+      <c r="H83" s="41"/>
+      <c r="I83" s="41"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="35"/>
-      <c r="B84" s="62"/>
-      <c r="C84" s="62"/>
+      <c r="A84" s="34"/>
+      <c r="B84" s="61"/>
+      <c r="C84" s="61"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="42"/>
-      <c r="H84" s="42"/>
-      <c r="I84" s="42"/>
+      <c r="G84" s="41"/>
+      <c r="H84" s="41"/>
+      <c r="I84" s="41"/>
     </row>
     <row r="85" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A85" s="35"/>
-      <c r="B85" s="63"/>
-      <c r="C85" s="63"/>
+      <c r="A85" s="34"/>
+      <c r="B85" s="62"/>
+      <c r="C85" s="62"/>
       <c r="D85" s="3"/>
-      <c r="E85" s="54"/>
+      <c r="E85" s="53"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="42"/>
-      <c r="H85" s="42"/>
-      <c r="I85" s="42"/>
+      <c r="G85" s="41"/>
+      <c r="H85" s="41"/>
+      <c r="I85" s="41"/>
     </row>
     <row r="86" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A86" s="35"/>
-      <c r="B86" s="63"/>
-      <c r="C86" s="63"/>
+      <c r="A86" s="34"/>
+      <c r="B86" s="62"/>
+      <c r="C86" s="62"/>
       <c r="D86" s="3"/>
-      <c r="E86" s="64"/>
-      <c r="F86" s="64"/>
-      <c r="G86" s="42"/>
-      <c r="H86" s="42"/>
-      <c r="I86" s="42"/>
+      <c r="E86" s="63"/>
+      <c r="F86" s="63"/>
+      <c r="G86" s="41"/>
+      <c r="H86" s="41"/>
+      <c r="I86" s="41"/>
     </row>
     <row r="87" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A87" s="35"/>
-      <c r="B87" s="63"/>
-      <c r="C87" s="63"/>
+      <c r="A87" s="34"/>
+      <c r="B87" s="62"/>
+      <c r="C87" s="62"/>
       <c r="D87" s="3"/>
-      <c r="E87" s="54"/>
+      <c r="E87" s="53"/>
       <c r="F87" s="3"/>
-      <c r="G87" s="42"/>
-      <c r="H87" s="42"/>
-      <c r="I87" s="42"/>
+      <c r="G87" s="41"/>
+      <c r="H87" s="41"/>
+      <c r="I87" s="41"/>
     </row>
     <row r="88" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A88" s="35"/>
-      <c r="B88" s="63"/>
-      <c r="C88" s="63"/>
+      <c r="A88" s="34"/>
+      <c r="B88" s="62"/>
+      <c r="C88" s="62"/>
       <c r="D88" s="3"/>
-      <c r="E88" s="54"/>
+      <c r="E88" s="53"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="42"/>
-      <c r="H88" s="42"/>
-      <c r="I88" s="42"/>
+      <c r="G88" s="41"/>
+      <c r="H88" s="41"/>
+      <c r="I88" s="41"/>
     </row>
     <row r="89" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A89" s="35"/>
-      <c r="B89" s="63"/>
-      <c r="C89" s="63"/>
+      <c r="A89" s="34"/>
+      <c r="B89" s="62"/>
+      <c r="C89" s="62"/>
       <c r="D89" s="3"/>
-      <c r="E89" s="54"/>
+      <c r="E89" s="53"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="42"/>
-      <c r="H89" s="42"/>
-      <c r="I89" s="42"/>
+      <c r="G89" s="41"/>
+      <c r="H89" s="41"/>
+      <c r="I89" s="41"/>
     </row>
     <row r="90" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A90" s="35"/>
-      <c r="B90" s="63"/>
-      <c r="C90" s="63"/>
+      <c r="A90" s="34"/>
+      <c r="B90" s="62"/>
+      <c r="C90" s="62"/>
       <c r="D90" s="3"/>
-      <c r="E90" s="54"/>
+      <c r="E90" s="53"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="42"/>
-      <c r="H90" s="42"/>
-      <c r="I90" s="42"/>
+      <c r="G90" s="41"/>
+      <c r="H90" s="41"/>
+      <c r="I90" s="41"/>
     </row>
     <row r="91" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A91" s="35"/>
-      <c r="B91" s="63"/>
-      <c r="C91" s="63"/>
+      <c r="A91" s="34"/>
+      <c r="B91" s="62"/>
+      <c r="C91" s="62"/>
       <c r="D91" s="3"/>
-      <c r="E91" s="54"/>
+      <c r="E91" s="53"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="42"/>
-      <c r="H91" s="42"/>
-      <c r="I91" s="42"/>
+      <c r="G91" s="41"/>
+      <c r="H91" s="41"/>
+      <c r="I91" s="41"/>
     </row>
     <row r="92" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A92" s="35"/>
-      <c r="B92" s="63"/>
-      <c r="C92" s="63"/>
+      <c r="A92" s="34"/>
+      <c r="B92" s="62"/>
+      <c r="C92" s="62"/>
       <c r="D92" s="3"/>
-      <c r="E92" s="54"/>
+      <c r="E92" s="53"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="42"/>
-      <c r="H92" s="42"/>
-      <c r="I92" s="42"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="41"/>
+      <c r="I92" s="41"/>
     </row>
     <row r="93" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A93" s="35"/>
-      <c r="B93" s="63"/>
-      <c r="C93" s="63"/>
+      <c r="A93" s="34"/>
+      <c r="B93" s="62"/>
+      <c r="C93" s="62"/>
       <c r="D93" s="3"/>
-      <c r="E93" s="54"/>
+      <c r="E93" s="53"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="42"/>
-      <c r="H93" s="42"/>
-      <c r="I93" s="42"/>
+      <c r="G93" s="41"/>
+      <c r="H93" s="41"/>
+      <c r="I93" s="41"/>
     </row>
     <row r="94" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A94" s="35"/>
-      <c r="B94" s="63"/>
-      <c r="C94" s="63"/>
+      <c r="A94" s="34"/>
+      <c r="B94" s="62"/>
+      <c r="C94" s="62"/>
       <c r="D94" s="3"/>
-      <c r="E94" s="54"/>
+      <c r="E94" s="53"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="42"/>
-      <c r="H94" s="42"/>
-      <c r="I94" s="42"/>
+      <c r="G94" s="41"/>
+      <c r="H94" s="41"/>
+      <c r="I94" s="41"/>
     </row>
     <row r="95" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A95" s="35"/>
-      <c r="B95" s="63"/>
-      <c r="C95" s="63"/>
+      <c r="A95" s="34"/>
+      <c r="B95" s="62"/>
+      <c r="C95" s="62"/>
       <c r="D95" s="3"/>
-      <c r="E95" s="54"/>
+      <c r="E95" s="53"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="42"/>
-      <c r="H95" s="42"/>
-      <c r="I95" s="42"/>
+      <c r="G95" s="41"/>
+      <c r="H95" s="41"/>
+      <c r="I95" s="41"/>
     </row>
     <row r="96" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A96" s="35"/>
-      <c r="B96" s="63"/>
-      <c r="C96" s="63"/>
+      <c r="A96" s="34"/>
+      <c r="B96" s="62"/>
+      <c r="C96" s="62"/>
       <c r="D96" s="3"/>
-      <c r="E96" s="54"/>
+      <c r="E96" s="53"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="42"/>
-      <c r="H96" s="42"/>
-      <c r="I96" s="42"/>
+      <c r="G96" s="41"/>
+      <c r="H96" s="41"/>
+      <c r="I96" s="41"/>
     </row>
     <row r="97" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A97" s="35"/>
-      <c r="B97" s="63"/>
-      <c r="C97" s="63"/>
+      <c r="A97" s="34"/>
+      <c r="B97" s="62"/>
+      <c r="C97" s="62"/>
       <c r="D97" s="3"/>
-      <c r="E97" s="54"/>
+      <c r="E97" s="53"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="42"/>
-      <c r="H97" s="42"/>
-      <c r="I97" s="42"/>
+      <c r="G97" s="41"/>
+      <c r="H97" s="41"/>
+      <c r="I97" s="41"/>
     </row>
     <row r="98" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A98" s="35"/>
-      <c r="B98" s="63"/>
-      <c r="C98" s="63"/>
+      <c r="A98" s="34"/>
+      <c r="B98" s="62"/>
+      <c r="C98" s="62"/>
       <c r="D98" s="3"/>
-      <c r="E98" s="54"/>
+      <c r="E98" s="53"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="42"/>
-      <c r="H98" s="42"/>
-      <c r="I98" s="42"/>
+      <c r="G98" s="41"/>
+      <c r="H98" s="41"/>
+      <c r="I98" s="41"/>
     </row>
     <row r="99" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A99" s="35"/>
-      <c r="B99" s="63"/>
-      <c r="C99" s="63"/>
+      <c r="A99" s="34"/>
+      <c r="B99" s="62"/>
+      <c r="C99" s="62"/>
       <c r="D99" s="3"/>
-      <c r="E99" s="54"/>
+      <c r="E99" s="53"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="42"/>
-      <c r="H99" s="42"/>
-      <c r="I99" s="42"/>
+      <c r="G99" s="41"/>
+      <c r="H99" s="41"/>
+      <c r="I99" s="41"/>
     </row>
     <row r="100" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A100" s="35"/>
-      <c r="B100" s="63"/>
-      <c r="C100" s="63"/>
+      <c r="A100" s="34"/>
+      <c r="B100" s="62"/>
+      <c r="C100" s="62"/>
       <c r="D100" s="3"/>
-      <c r="E100" s="54"/>
+      <c r="E100" s="53"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="42"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="42"/>
+      <c r="G100" s="41"/>
+      <c r="H100" s="41"/>
+      <c r="I100" s="41"/>
     </row>
     <row r="101" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A101" s="35"/>
-      <c r="B101" s="63"/>
-      <c r="C101" s="63"/>
+      <c r="A101" s="34"/>
+      <c r="B101" s="62"/>
+      <c r="C101" s="62"/>
       <c r="D101" s="3"/>
-      <c r="E101" s="95"/>
-      <c r="F101" s="95"/>
-      <c r="G101" s="42"/>
-      <c r="H101" s="42"/>
-      <c r="I101" s="42"/>
+      <c r="E101" s="120"/>
+      <c r="F101" s="120"/>
+      <c r="G101" s="41"/>
+      <c r="H101" s="41"/>
+      <c r="I101" s="41"/>
     </row>
     <row r="102" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A102" s="35"/>
-      <c r="B102" s="63"/>
-      <c r="C102" s="63"/>
+      <c r="A102" s="34"/>
+      <c r="B102" s="62"/>
+      <c r="C102" s="62"/>
       <c r="D102" s="3"/>
-      <c r="E102" s="54"/>
+      <c r="E102" s="53"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="42"/>
-      <c r="H102" s="42"/>
-      <c r="I102" s="42"/>
+      <c r="G102" s="41"/>
+      <c r="H102" s="41"/>
+      <c r="I102" s="41"/>
     </row>
     <row r="103" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A103" s="35"/>
-      <c r="B103" s="63"/>
-      <c r="C103" s="63"/>
+      <c r="A103" s="34"/>
+      <c r="B103" s="62"/>
+      <c r="C103" s="62"/>
       <c r="D103" s="3"/>
-      <c r="E103" s="65"/>
+      <c r="E103" s="64"/>
       <c r="F103" s="3"/>
-      <c r="G103" s="42"/>
-      <c r="H103" s="42"/>
-      <c r="I103" s="42"/>
+      <c r="G103" s="41"/>
+      <c r="H103" s="41"/>
+      <c r="I103" s="41"/>
     </row>
     <row r="104" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A104" s="35"/>
-      <c r="B104" s="63"/>
-      <c r="C104" s="63"/>
+      <c r="A104" s="34"/>
+      <c r="B104" s="62"/>
+      <c r="C104" s="62"/>
       <c r="D104" s="3"/>
-      <c r="E104" s="65"/>
+      <c r="E104" s="64"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="42"/>
-      <c r="H104" s="42"/>
-      <c r="I104" s="42"/>
+      <c r="G104" s="41"/>
+      <c r="H104" s="41"/>
+      <c r="I104" s="41"/>
     </row>
     <row r="105" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A105" s="35"/>
-      <c r="B105" s="63"/>
-      <c r="C105" s="63"/>
+      <c r="A105" s="34"/>
+      <c r="B105" s="62"/>
+      <c r="C105" s="62"/>
       <c r="D105" s="3"/>
-      <c r="E105" s="66"/>
+      <c r="E105" s="65"/>
       <c r="F105" s="3"/>
-      <c r="G105" s="42"/>
-      <c r="H105" s="42"/>
-      <c r="I105" s="42"/>
+      <c r="G105" s="41"/>
+      <c r="H105" s="41"/>
+      <c r="I105" s="41"/>
     </row>
     <row r="106" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A106" s="35"/>
-      <c r="B106" s="63"/>
-      <c r="C106" s="63"/>
+      <c r="A106" s="34"/>
+      <c r="B106" s="62"/>
+      <c r="C106" s="62"/>
       <c r="D106" s="3"/>
-      <c r="E106" s="66"/>
+      <c r="E106" s="65"/>
       <c r="F106" s="3"/>
-      <c r="G106" s="42"/>
-      <c r="H106" s="42"/>
-      <c r="I106" s="42"/>
+      <c r="G106" s="41"/>
+      <c r="H106" s="41"/>
+      <c r="I106" s="41"/>
     </row>
     <row r="107" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A107" s="35"/>
-      <c r="B107" s="63"/>
-      <c r="C107" s="63"/>
+      <c r="A107" s="34"/>
+      <c r="B107" s="62"/>
+      <c r="C107" s="62"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
-      <c r="G107" s="42"/>
-      <c r="H107" s="42"/>
-      <c r="I107" s="42"/>
+      <c r="G107" s="41"/>
+      <c r="H107" s="41"/>
+      <c r="I107" s="41"/>
     </row>
     <row r="108" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A108" s="35"/>
-      <c r="B108" s="63"/>
-      <c r="C108" s="63"/>
+      <c r="A108" s="34"/>
+      <c r="B108" s="62"/>
+      <c r="C108" s="62"/>
       <c r="D108" s="3"/>
-      <c r="E108" s="67"/>
-      <c r="F108" s="54"/>
-      <c r="G108" s="42"/>
-      <c r="H108" s="42"/>
-      <c r="I108" s="42"/>
+      <c r="E108" s="66"/>
+      <c r="F108" s="53"/>
+      <c r="G108" s="41"/>
+      <c r="H108" s="41"/>
+      <c r="I108" s="41"/>
     </row>
     <row r="109" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A109" s="35"/>
-      <c r="B109" s="63"/>
-      <c r="C109" s="63"/>
+      <c r="A109" s="34"/>
+      <c r="B109" s="62"/>
+      <c r="C109" s="62"/>
       <c r="D109" s="3"/>
-      <c r="E109" s="67"/>
-      <c r="F109" s="54"/>
-      <c r="G109" s="42"/>
-      <c r="H109" s="42"/>
-      <c r="I109" s="42"/>
+      <c r="E109" s="66"/>
+      <c r="F109" s="53"/>
+      <c r="G109" s="41"/>
+      <c r="H109" s="41"/>
+      <c r="I109" s="41"/>
     </row>
     <row r="110" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A110" s="35"/>
-      <c r="B110" s="63"/>
-      <c r="C110" s="63"/>
+      <c r="A110" s="34"/>
+      <c r="B110" s="62"/>
+      <c r="C110" s="62"/>
       <c r="D110" s="3"/>
-      <c r="E110" s="67"/>
-      <c r="F110" s="54"/>
-      <c r="G110" s="42"/>
-      <c r="H110" s="42"/>
-      <c r="I110" s="42"/>
+      <c r="E110" s="66"/>
+      <c r="F110" s="53"/>
+      <c r="G110" s="41"/>
+      <c r="H110" s="41"/>
+      <c r="I110" s="41"/>
     </row>
     <row r="111" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A111" s="35"/>
-      <c r="B111" s="63"/>
-      <c r="C111" s="63"/>
+      <c r="A111" s="34"/>
+      <c r="B111" s="62"/>
+      <c r="C111" s="62"/>
       <c r="D111" s="3"/>
-      <c r="E111" s="67"/>
-      <c r="F111" s="54"/>
-      <c r="G111" s="42"/>
-      <c r="H111" s="42"/>
-      <c r="I111" s="42"/>
+      <c r="E111" s="66"/>
+      <c r="F111" s="53"/>
+      <c r="G111" s="41"/>
+      <c r="H111" s="41"/>
+      <c r="I111" s="41"/>
     </row>
     <row r="112" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A112" s="35"/>
-      <c r="B112" s="63"/>
-      <c r="C112" s="63"/>
+      <c r="A112" s="34"/>
+      <c r="B112" s="62"/>
+      <c r="C112" s="62"/>
       <c r="D112" s="3"/>
-      <c r="E112" s="67"/>
-      <c r="F112" s="54"/>
-      <c r="G112" s="42"/>
-      <c r="H112" s="42"/>
-      <c r="I112" s="42"/>
+      <c r="E112" s="66"/>
+      <c r="F112" s="53"/>
+      <c r="G112" s="41"/>
+      <c r="H112" s="41"/>
+      <c r="I112" s="41"/>
     </row>
     <row r="113" spans="1:9" ht="18" customHeight="1">
-      <c r="A113" s="35"/>
-      <c r="B113" s="63"/>
-      <c r="C113" s="63"/>
+      <c r="A113" s="34"/>
+      <c r="B113" s="62"/>
+      <c r="C113" s="62"/>
       <c r="D113" s="3"/>
-      <c r="E113" s="67"/>
-      <c r="F113" s="54"/>
-      <c r="G113" s="42"/>
-      <c r="H113" s="42"/>
-      <c r="I113" s="42"/>
+      <c r="E113" s="66"/>
+      <c r="F113" s="53"/>
+      <c r="G113" s="41"/>
+      <c r="H113" s="41"/>
+      <c r="I113" s="41"/>
     </row>
     <row r="114" spans="1:9" ht="18" customHeight="1">
-      <c r="A114" s="35"/>
-      <c r="B114" s="63"/>
-      <c r="C114" s="63"/>
+      <c r="A114" s="34"/>
+      <c r="B114" s="62"/>
+      <c r="C114" s="62"/>
       <c r="D114" s="3"/>
-      <c r="E114" s="66"/>
+      <c r="E114" s="65"/>
       <c r="F114" s="3"/>
-      <c r="G114" s="42"/>
-      <c r="H114" s="42"/>
-      <c r="I114" s="42"/>
+      <c r="G114" s="41"/>
+      <c r="H114" s="41"/>
+      <c r="I114" s="41"/>
     </row>
     <row r="115" spans="1:9" ht="18" customHeight="1">
-      <c r="A115" s="35"/>
-      <c r="B115" s="63"/>
-      <c r="C115" s="63"/>
+      <c r="A115" s="34"/>
+      <c r="B115" s="62"/>
+      <c r="C115" s="62"/>
       <c r="D115" s="3"/>
-      <c r="E115" s="66"/>
+      <c r="E115" s="65"/>
       <c r="F115" s="3"/>
-      <c r="G115" s="42"/>
-      <c r="H115" s="42"/>
-      <c r="I115" s="42"/>
+      <c r="G115" s="41"/>
+      <c r="H115" s="41"/>
+      <c r="I115" s="41"/>
     </row>
     <row r="116" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A116" s="35"/>
-      <c r="B116" s="63"/>
-      <c r="C116" s="63"/>
+      <c r="A116" s="34"/>
+      <c r="B116" s="62"/>
+      <c r="C116" s="62"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
-      <c r="G116" s="42"/>
-      <c r="H116" s="42"/>
-      <c r="I116" s="42"/>
+      <c r="G116" s="41"/>
+      <c r="H116" s="41"/>
+      <c r="I116" s="41"/>
     </row>
     <row r="117" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A117" s="35"/>
-      <c r="B117" s="63"/>
-      <c r="C117" s="63"/>
+      <c r="A117" s="34"/>
+      <c r="B117" s="62"/>
+      <c r="C117" s="62"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="4"/>
-      <c r="G117" s="42"/>
-      <c r="H117" s="42"/>
-      <c r="I117" s="42"/>
+      <c r="G117" s="41"/>
+      <c r="H117" s="41"/>
+      <c r="I117" s="41"/>
     </row>
     <row r="118" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A118" s="35"/>
-      <c r="B118" s="63"/>
-      <c r="C118" s="63"/>
+      <c r="A118" s="34"/>
+      <c r="B118" s="62"/>
+      <c r="C118" s="62"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
-      <c r="G118" s="42"/>
-      <c r="H118" s="42"/>
-      <c r="I118" s="42"/>
+      <c r="G118" s="41"/>
+      <c r="H118" s="41"/>
+      <c r="I118" s="41"/>
     </row>
     <row r="119" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A119" s="35"/>
-      <c r="B119" s="63"/>
-      <c r="C119" s="63"/>
+      <c r="A119" s="34"/>
+      <c r="B119" s="62"/>
+      <c r="C119" s="62"/>
       <c r="D119" s="3"/>
-      <c r="E119" s="66"/>
+      <c r="E119" s="65"/>
       <c r="F119" s="3"/>
-      <c r="G119" s="42"/>
-      <c r="H119" s="42"/>
-      <c r="I119" s="42"/>
+      <c r="G119" s="41"/>
+      <c r="H119" s="41"/>
+      <c r="I119" s="41"/>
     </row>
     <row r="120" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A120" s="35"/>
-      <c r="B120" s="68"/>
-      <c r="C120" s="68"/>
+      <c r="A120" s="34"/>
+      <c r="B120" s="67"/>
+      <c r="C120" s="67"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="42"/>
-      <c r="H120" s="42"/>
-      <c r="I120" s="42"/>
+      <c r="G120" s="41"/>
+      <c r="H120" s="41"/>
+      <c r="I120" s="41"/>
     </row>
     <row r="121" spans="1:9" ht="15" customHeight="1">
-      <c r="A121" s="35"/>
-      <c r="B121" s="59"/>
-      <c r="C121" s="59"/>
+      <c r="A121" s="34"/>
+      <c r="B121" s="58"/>
+      <c r="C121" s="58"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
-      <c r="G121" s="42"/>
-      <c r="H121" s="42"/>
-      <c r="I121" s="42"/>
+      <c r="G121" s="41"/>
+      <c r="H121" s="41"/>
+      <c r="I121" s="41"/>
     </row>
     <row r="122" spans="1:9" ht="15" customHeight="1">
-      <c r="A122" s="35"/>
-      <c r="B122" s="59"/>
-      <c r="C122" s="59"/>
+      <c r="A122" s="34"/>
+      <c r="B122" s="58"/>
+      <c r="C122" s="58"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
-      <c r="G122" s="42"/>
-      <c r="H122" s="42"/>
-      <c r="I122" s="42"/>
+      <c r="G122" s="41"/>
+      <c r="H122" s="41"/>
+      <c r="I122" s="41"/>
     </row>
     <row r="123" spans="1:9" ht="15" customHeight="1">
-      <c r="A123" s="35"/>
-      <c r="B123" s="59"/>
-      <c r="C123" s="59"/>
+      <c r="A123" s="34"/>
+      <c r="B123" s="58"/>
+      <c r="C123" s="58"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
-      <c r="G123" s="42"/>
-      <c r="H123" s="42"/>
-      <c r="I123" s="42"/>
+      <c r="G123" s="41"/>
+      <c r="H123" s="41"/>
+      <c r="I123" s="41"/>
     </row>
     <row r="124" spans="1:9">
-      <c r="A124" s="56"/>
-      <c r="B124" s="56"/>
-      <c r="C124" s="56"/>
-      <c r="D124" s="56"/>
-      <c r="E124" s="69"/>
-      <c r="F124" s="69"/>
-      <c r="G124" s="42"/>
-      <c r="H124" s="42"/>
-      <c r="I124" s="42"/>
+      <c r="A124" s="55"/>
+      <c r="B124" s="55"/>
+      <c r="C124" s="55"/>
+      <c r="D124" s="55"/>
+      <c r="E124" s="68"/>
+      <c r="F124" s="68"/>
+      <c r="G124" s="41"/>
+      <c r="H124" s="41"/>
+      <c r="I124" s="41"/>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="3"/>
@@ -2937,7 +2945,7 @@
       <c r="F125" s="3"/>
     </row>
     <row r="126" spans="1:9" ht="13.5">
-      <c r="A126" s="59"/>
+      <c r="A126" s="58"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
@@ -2953,7 +2961,7 @@
       <c r="F127" s="3"/>
     </row>
     <row r="128" spans="1:9" ht="13.5">
-      <c r="A128" s="59"/>
+      <c r="A128" s="58"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
@@ -2962,238 +2970,238 @@
     </row>
     <row r="129" spans="1:6" ht="13.5">
       <c r="A129" s="3"/>
-      <c r="B129" s="70"/>
-      <c r="C129" s="70"/>
+      <c r="B129" s="69"/>
+      <c r="C129" s="69"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
     </row>
     <row r="130" spans="1:6" ht="30.75" customHeight="1">
       <c r="A130" s="3"/>
-      <c r="B130" s="97"/>
-      <c r="C130" s="97"/>
-      <c r="D130" s="97"/>
-      <c r="E130" s="97"/>
-      <c r="F130" s="97"/>
+      <c r="B130" s="121"/>
+      <c r="C130" s="121"/>
+      <c r="D130" s="121"/>
+      <c r="E130" s="121"/>
+      <c r="F130" s="121"/>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="3"/>
-      <c r="B131" s="71"/>
-      <c r="C131" s="71"/>
-      <c r="D131" s="71"/>
-      <c r="E131" s="71"/>
-      <c r="F131" s="71"/>
+      <c r="B131" s="70"/>
+      <c r="C131" s="70"/>
+      <c r="D131" s="70"/>
+      <c r="E131" s="70"/>
+      <c r="F131" s="70"/>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="3"/>
-      <c r="B132" s="72"/>
-      <c r="C132" s="72"/>
-      <c r="D132" s="91"/>
-      <c r="E132" s="91"/>
-      <c r="F132" s="91"/>
+      <c r="B132" s="71"/>
+      <c r="C132" s="71"/>
+      <c r="D132" s="119"/>
+      <c r="E132" s="119"/>
+      <c r="F132" s="119"/>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" s="3"/>
-      <c r="B133" s="73"/>
-      <c r="C133" s="73"/>
-      <c r="D133" s="71"/>
-      <c r="E133" s="71"/>
-      <c r="F133" s="71"/>
+      <c r="B133" s="72"/>
+      <c r="C133" s="72"/>
+      <c r="D133" s="70"/>
+      <c r="E133" s="70"/>
+      <c r="F133" s="70"/>
     </row>
     <row r="134" spans="1:6" ht="49.5" customHeight="1">
       <c r="A134" s="3"/>
-      <c r="B134" s="74"/>
-      <c r="C134" s="74"/>
-      <c r="D134" s="93"/>
-      <c r="E134" s="91"/>
-      <c r="F134" s="91"/>
+      <c r="B134" s="73"/>
+      <c r="C134" s="73"/>
+      <c r="D134" s="118"/>
+      <c r="E134" s="119"/>
+      <c r="F134" s="119"/>
     </row>
     <row r="135" spans="1:6">
       <c r="A135" s="3"/>
-      <c r="B135" s="75"/>
-      <c r="C135" s="75"/>
-      <c r="D135" s="71"/>
-      <c r="E135" s="71"/>
-      <c r="F135" s="71"/>
+      <c r="B135" s="74"/>
+      <c r="C135" s="74"/>
+      <c r="D135" s="70"/>
+      <c r="E135" s="70"/>
+      <c r="F135" s="70"/>
     </row>
     <row r="136" spans="1:6">
       <c r="A136" s="3"/>
-      <c r="B136" s="72"/>
-      <c r="C136" s="72"/>
-      <c r="D136" s="91"/>
-      <c r="E136" s="91"/>
-      <c r="F136" s="91"/>
+      <c r="B136" s="71"/>
+      <c r="C136" s="71"/>
+      <c r="D136" s="119"/>
+      <c r="E136" s="119"/>
+      <c r="F136" s="119"/>
     </row>
     <row r="137" spans="1:6">
       <c r="A137" s="3"/>
-      <c r="B137" s="73"/>
-      <c r="C137" s="73"/>
-      <c r="D137" s="71"/>
-      <c r="E137" s="71"/>
-      <c r="F137" s="71"/>
+      <c r="B137" s="72"/>
+      <c r="C137" s="72"/>
+      <c r="D137" s="70"/>
+      <c r="E137" s="70"/>
+      <c r="F137" s="70"/>
     </row>
     <row r="138" spans="1:6" ht="78.75" customHeight="1">
       <c r="A138" s="3"/>
-      <c r="B138" s="74"/>
-      <c r="C138" s="74"/>
-      <c r="D138" s="93"/>
-      <c r="E138" s="91"/>
-      <c r="F138" s="91"/>
+      <c r="B138" s="73"/>
+      <c r="C138" s="73"/>
+      <c r="D138" s="118"/>
+      <c r="E138" s="119"/>
+      <c r="F138" s="119"/>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="3"/>
-      <c r="B139" s="73"/>
-      <c r="C139" s="73"/>
-      <c r="D139" s="71"/>
-      <c r="E139" s="71"/>
-      <c r="F139" s="71"/>
+      <c r="B139" s="72"/>
+      <c r="C139" s="72"/>
+      <c r="D139" s="70"/>
+      <c r="E139" s="70"/>
+      <c r="F139" s="70"/>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="3"/>
-      <c r="B140" s="73"/>
-      <c r="C140" s="73"/>
-      <c r="D140" s="71"/>
-      <c r="E140" s="71"/>
-      <c r="F140" s="71"/>
+      <c r="B140" s="72"/>
+      <c r="C140" s="72"/>
+      <c r="D140" s="70"/>
+      <c r="E140" s="70"/>
+      <c r="F140" s="70"/>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="3"/>
-      <c r="B141" s="72"/>
-      <c r="C141" s="72"/>
-      <c r="D141" s="91"/>
-      <c r="E141" s="91"/>
-      <c r="F141" s="91"/>
+      <c r="B141" s="71"/>
+      <c r="C141" s="71"/>
+      <c r="D141" s="119"/>
+      <c r="E141" s="119"/>
+      <c r="F141" s="119"/>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="3"/>
-      <c r="B142" s="71"/>
-      <c r="C142" s="71"/>
-      <c r="D142" s="71"/>
-      <c r="E142" s="71"/>
-      <c r="F142" s="71"/>
+      <c r="B142" s="70"/>
+      <c r="C142" s="70"/>
+      <c r="D142" s="70"/>
+      <c r="E142" s="70"/>
+      <c r="F142" s="70"/>
     </row>
     <row r="143" spans="1:6" ht="58.5" customHeight="1">
       <c r="A143" s="3"/>
-      <c r="B143" s="74"/>
-      <c r="C143" s="74"/>
-      <c r="D143" s="93"/>
-      <c r="E143" s="91"/>
-      <c r="F143" s="91"/>
+      <c r="B143" s="73"/>
+      <c r="C143" s="73"/>
+      <c r="D143" s="118"/>
+      <c r="E143" s="119"/>
+      <c r="F143" s="119"/>
     </row>
     <row r="144" spans="1:6" ht="90" customHeight="1">
       <c r="A144" s="3"/>
-      <c r="B144" s="74"/>
-      <c r="C144" s="74"/>
-      <c r="D144" s="93"/>
-      <c r="E144" s="91"/>
-      <c r="F144" s="91"/>
+      <c r="B144" s="73"/>
+      <c r="C144" s="73"/>
+      <c r="D144" s="118"/>
+      <c r="E144" s="119"/>
+      <c r="F144" s="119"/>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="3"/>
-      <c r="B145" s="74"/>
-      <c r="C145" s="74"/>
-      <c r="D145" s="94"/>
-      <c r="E145" s="95"/>
-      <c r="F145" s="95"/>
+      <c r="B145" s="73"/>
+      <c r="C145" s="73"/>
+      <c r="D145" s="123"/>
+      <c r="E145" s="120"/>
+      <c r="F145" s="120"/>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="3"/>
-      <c r="B146" s="76"/>
-      <c r="C146" s="76"/>
-      <c r="D146" s="90"/>
-      <c r="E146" s="90"/>
-      <c r="F146" s="77"/>
+      <c r="B146" s="75"/>
+      <c r="C146" s="75"/>
+      <c r="D146" s="122"/>
+      <c r="E146" s="122"/>
+      <c r="F146" s="76"/>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" s="3"/>
-      <c r="B147" s="76"/>
-      <c r="C147" s="76"/>
-      <c r="D147" s="90"/>
-      <c r="E147" s="90"/>
-      <c r="F147" s="77"/>
+      <c r="B147" s="75"/>
+      <c r="C147" s="75"/>
+      <c r="D147" s="122"/>
+      <c r="E147" s="122"/>
+      <c r="F147" s="76"/>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="3"/>
-      <c r="B148" s="76"/>
-      <c r="C148" s="76"/>
-      <c r="D148" s="90"/>
-      <c r="E148" s="90"/>
-      <c r="F148" s="77"/>
+      <c r="B148" s="75"/>
+      <c r="C148" s="75"/>
+      <c r="D148" s="122"/>
+      <c r="E148" s="122"/>
+      <c r="F148" s="76"/>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="3"/>
-      <c r="B149" s="76"/>
-      <c r="C149" s="76"/>
-      <c r="D149" s="90"/>
-      <c r="E149" s="90"/>
-      <c r="F149" s="77"/>
+      <c r="B149" s="75"/>
+      <c r="C149" s="75"/>
+      <c r="D149" s="122"/>
+      <c r="E149" s="122"/>
+      <c r="F149" s="76"/>
     </row>
     <row r="150" spans="1:6">
       <c r="A150" s="3"/>
-      <c r="B150" s="76"/>
-      <c r="C150" s="76"/>
-      <c r="D150" s="90"/>
-      <c r="E150" s="90"/>
-      <c r="F150" s="77"/>
+      <c r="B150" s="75"/>
+      <c r="C150" s="75"/>
+      <c r="D150" s="122"/>
+      <c r="E150" s="122"/>
+      <c r="F150" s="76"/>
     </row>
     <row r="151" spans="1:6">
       <c r="A151" s="3"/>
-      <c r="B151" s="76"/>
-      <c r="C151" s="76"/>
-      <c r="D151" s="90"/>
-      <c r="E151" s="90"/>
-      <c r="F151" s="77"/>
+      <c r="B151" s="75"/>
+      <c r="C151" s="75"/>
+      <c r="D151" s="122"/>
+      <c r="E151" s="122"/>
+      <c r="F151" s="76"/>
     </row>
     <row r="152" spans="1:6">
       <c r="A152" s="3"/>
-      <c r="B152" s="76"/>
-      <c r="C152" s="76"/>
-      <c r="D152" s="90"/>
-      <c r="E152" s="90"/>
-      <c r="F152" s="78"/>
+      <c r="B152" s="75"/>
+      <c r="C152" s="75"/>
+      <c r="D152" s="122"/>
+      <c r="E152" s="122"/>
+      <c r="F152" s="77"/>
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="3"/>
-      <c r="B153" s="76"/>
-      <c r="C153" s="76"/>
-      <c r="D153" s="90"/>
-      <c r="E153" s="90"/>
-      <c r="F153" s="78"/>
+      <c r="B153" s="75"/>
+      <c r="C153" s="75"/>
+      <c r="D153" s="122"/>
+      <c r="E153" s="122"/>
+      <c r="F153" s="77"/>
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="3"/>
-      <c r="B154" s="76"/>
-      <c r="C154" s="76"/>
-      <c r="D154" s="90"/>
-      <c r="E154" s="90"/>
-      <c r="F154" s="78"/>
+      <c r="B154" s="75"/>
+      <c r="C154" s="75"/>
+      <c r="D154" s="122"/>
+      <c r="E154" s="122"/>
+      <c r="F154" s="77"/>
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="3"/>
-      <c r="B155" s="76"/>
-      <c r="C155" s="76"/>
-      <c r="D155" s="90"/>
-      <c r="E155" s="90"/>
-      <c r="F155" s="78"/>
+      <c r="B155" s="75"/>
+      <c r="C155" s="75"/>
+      <c r="D155" s="122"/>
+      <c r="E155" s="122"/>
+      <c r="F155" s="77"/>
     </row>
     <row r="156" spans="1:6" ht="26.25" customHeight="1">
       <c r="A156" s="3"/>
-      <c r="B156" s="76"/>
-      <c r="C156" s="76"/>
-      <c r="D156" s="92"/>
-      <c r="E156" s="92"/>
-      <c r="F156" s="92"/>
+      <c r="B156" s="75"/>
+      <c r="C156" s="75"/>
+      <c r="D156" s="124"/>
+      <c r="E156" s="124"/>
+      <c r="F156" s="124"/>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
-      <c r="D157" s="79"/>
+      <c r="D157" s="78"/>
       <c r="E157" s="3"/>
       <c r="F157" s="3"/>
     </row>
     <row r="158" spans="1:6" ht="13.5">
-      <c r="A158" s="59"/>
+      <c r="A158" s="58"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
@@ -3209,7 +3217,7 @@
       <c r="F159" s="3"/>
     </row>
     <row r="160" spans="1:6">
-      <c r="A160" s="74"/>
+      <c r="A160" s="73"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
@@ -3217,7 +3225,7 @@
       <c r="F160" s="3"/>
     </row>
     <row r="161" spans="1:6">
-      <c r="A161" s="74"/>
+      <c r="A161" s="73"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
@@ -3225,7 +3233,7 @@
       <c r="F161" s="3"/>
     </row>
     <row r="162" spans="1:6">
-      <c r="A162" s="74"/>
+      <c r="A162" s="73"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
@@ -3234,123 +3242,123 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="3"/>
-      <c r="B163" s="90"/>
-      <c r="C163" s="90"/>
-      <c r="D163" s="90"/>
+      <c r="B163" s="122"/>
+      <c r="C163" s="122"/>
+      <c r="D163" s="122"/>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="3"/>
-      <c r="B164" s="90"/>
-      <c r="C164" s="90"/>
-      <c r="D164" s="90"/>
+      <c r="B164" s="122"/>
+      <c r="C164" s="122"/>
+      <c r="D164" s="122"/>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="3"/>
-      <c r="B165" s="90"/>
-      <c r="C165" s="90"/>
-      <c r="D165" s="90"/>
+      <c r="B165" s="122"/>
+      <c r="C165" s="122"/>
+      <c r="D165" s="122"/>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="3"/>
-      <c r="B166" s="90"/>
-      <c r="C166" s="90"/>
-      <c r="D166" s="90"/>
+      <c r="B166" s="122"/>
+      <c r="C166" s="122"/>
+      <c r="D166" s="122"/>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="3"/>
-      <c r="B167" s="90"/>
-      <c r="C167" s="90"/>
-      <c r="D167" s="90"/>
+      <c r="B167" s="122"/>
+      <c r="C167" s="122"/>
+      <c r="D167" s="122"/>
       <c r="E167" s="3"/>
       <c r="F167" s="3"/>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="3"/>
-      <c r="B168" s="90"/>
-      <c r="C168" s="90"/>
-      <c r="D168" s="90"/>
+      <c r="B168" s="122"/>
+      <c r="C168" s="122"/>
+      <c r="D168" s="122"/>
       <c r="E168" s="3"/>
       <c r="F168" s="3"/>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="3"/>
-      <c r="B169" s="90"/>
-      <c r="C169" s="90"/>
-      <c r="D169" s="90"/>
+      <c r="B169" s="122"/>
+      <c r="C169" s="122"/>
+      <c r="D169" s="122"/>
       <c r="E169" s="3"/>
       <c r="F169" s="3"/>
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="3"/>
-      <c r="B170" s="90"/>
-      <c r="C170" s="90"/>
-      <c r="D170" s="90"/>
+      <c r="B170" s="122"/>
+      <c r="C170" s="122"/>
+      <c r="D170" s="122"/>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="3"/>
-      <c r="B171" s="90"/>
-      <c r="C171" s="90"/>
-      <c r="D171" s="90"/>
+      <c r="B171" s="122"/>
+      <c r="C171" s="122"/>
+      <c r="D171" s="122"/>
       <c r="E171" s="3"/>
       <c r="F171" s="3"/>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="3"/>
-      <c r="B172" s="90"/>
-      <c r="C172" s="90"/>
-      <c r="D172" s="90"/>
+      <c r="B172" s="122"/>
+      <c r="C172" s="122"/>
+      <c r="D172" s="122"/>
       <c r="E172" s="3"/>
       <c r="F172" s="3"/>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="3"/>
-      <c r="B173" s="90"/>
-      <c r="C173" s="90"/>
-      <c r="D173" s="90"/>
+      <c r="B173" s="122"/>
+      <c r="C173" s="122"/>
+      <c r="D173" s="122"/>
       <c r="E173" s="3"/>
       <c r="F173" s="3"/>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="3"/>
-      <c r="B174" s="90"/>
-      <c r="C174" s="90"/>
-      <c r="D174" s="90"/>
+      <c r="B174" s="122"/>
+      <c r="C174" s="122"/>
+      <c r="D174" s="122"/>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
     </row>
     <row r="175" spans="1:6">
-      <c r="A175" s="74"/>
+      <c r="A175" s="73"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
-      <c r="D175" s="80"/>
+      <c r="D175" s="79"/>
       <c r="E175" s="3"/>
       <c r="F175" s="3"/>
     </row>
     <row r="176" spans="1:6" ht="15" customHeight="1">
-      <c r="A176" s="74"/>
-      <c r="B176" s="91"/>
-      <c r="C176" s="91"/>
-      <c r="D176" s="91"/>
-      <c r="E176" s="91"/>
-      <c r="F176" s="91"/>
+      <c r="A176" s="73"/>
+      <c r="B176" s="119"/>
+      <c r="C176" s="119"/>
+      <c r="D176" s="119"/>
+      <c r="E176" s="119"/>
+      <c r="F176" s="119"/>
     </row>
     <row r="177" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A177" s="74"/>
-      <c r="B177" s="91"/>
-      <c r="C177" s="91"/>
-      <c r="D177" s="91"/>
-      <c r="E177" s="91"/>
-      <c r="F177" s="91"/>
+      <c r="A177" s="73"/>
+      <c r="B177" s="119"/>
+      <c r="C177" s="119"/>
+      <c r="D177" s="119"/>
+      <c r="E177" s="119"/>
+      <c r="F177" s="119"/>
     </row>
     <row r="178" spans="1:6">
       <c r="A178" s="3"/>
@@ -3361,7 +3369,7 @@
       <c r="F178" s="3"/>
     </row>
     <row r="179" spans="1:6" ht="13.5">
-      <c r="A179" s="59"/>
+      <c r="A179" s="58"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
@@ -3377,46 +3385,113 @@
       <c r="F180" s="3"/>
     </row>
     <row r="181" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A181" s="74"/>
-      <c r="B181" s="89"/>
-      <c r="C181" s="89"/>
-      <c r="D181" s="89"/>
-      <c r="E181" s="89"/>
-      <c r="F181" s="89"/>
+      <c r="A181" s="73"/>
+      <c r="B181" s="125"/>
+      <c r="C181" s="125"/>
+      <c r="D181" s="125"/>
+      <c r="E181" s="125"/>
+      <c r="F181" s="125"/>
     </row>
     <row r="182" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A182" s="74"/>
-      <c r="B182" s="89"/>
-      <c r="C182" s="89"/>
-      <c r="D182" s="89"/>
-      <c r="E182" s="89"/>
-      <c r="F182" s="89"/>
+      <c r="A182" s="73"/>
+      <c r="B182" s="125"/>
+      <c r="C182" s="125"/>
+      <c r="D182" s="125"/>
+      <c r="E182" s="125"/>
+      <c r="F182" s="125"/>
     </row>
     <row r="183" spans="1:6" ht="18" customHeight="1">
-      <c r="A183" s="74"/>
-      <c r="B183" s="89"/>
-      <c r="C183" s="89"/>
-      <c r="D183" s="89"/>
-      <c r="E183" s="89"/>
-      <c r="F183" s="89"/>
+      <c r="A183" s="73"/>
+      <c r="B183" s="125"/>
+      <c r="C183" s="125"/>
+      <c r="D183" s="125"/>
+      <c r="E183" s="125"/>
+      <c r="F183" s="125"/>
     </row>
     <row r="184" spans="1:6">
-      <c r="A184" s="74"/>
-      <c r="B184" s="89"/>
-      <c r="C184" s="89"/>
-      <c r="D184" s="89"/>
-      <c r="E184" s="89"/>
-      <c r="F184" s="89"/>
+      <c r="A184" s="73"/>
+      <c r="B184" s="125"/>
+      <c r="C184" s="125"/>
+      <c r="D184" s="125"/>
+      <c r="E184" s="125"/>
+      <c r="F184" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B174:D174"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B173:D173"/>
+    <mergeCell ref="D156:F156"/>
+    <mergeCell ref="B163:D163"/>
+    <mergeCell ref="B164:D164"/>
+    <mergeCell ref="B165:D165"/>
+    <mergeCell ref="B166:D166"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="B168:D168"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="B171:D171"/>
+    <mergeCell ref="B172:D172"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D144:F144"/>
+    <mergeCell ref="D145:F145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="D132:F132"/>
+    <mergeCell ref="D134:F134"/>
+    <mergeCell ref="D136:F136"/>
+    <mergeCell ref="D138:F138"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="B13:C13"/>
@@ -3430,80 +3505,13 @@
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="D132:F132"/>
-    <mergeCell ref="D134:F134"/>
-    <mergeCell ref="D136:F136"/>
-    <mergeCell ref="D138:F138"/>
-    <mergeCell ref="D141:F141"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D144:F144"/>
-    <mergeCell ref="D145:F145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="B173:D173"/>
-    <mergeCell ref="D156:F156"/>
-    <mergeCell ref="B163:D163"/>
-    <mergeCell ref="B164:D164"/>
-    <mergeCell ref="B165:D165"/>
-    <mergeCell ref="B166:D166"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="B168:D168"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="B171:D171"/>
-    <mergeCell ref="B172:D172"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B174:D174"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="B69:C70">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -3528,114 +3536,114 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:J4"/>
+      <selection activeCell="C2" sqref="C2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="82" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="82" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="82" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="82" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="82" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="82" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="82" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="82" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="82" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="82" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="22.5703125" style="82"/>
+    <col min="1" max="1" width="2.5703125" style="81" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="81" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="81" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="81" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="81" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="81" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="81" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="81" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="81" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="22.5703125" style="81"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="48" customHeight="1">
-      <c r="B2" s="81"/>
-      <c r="C2" s="127" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="126" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
     </row>
     <row r="3" spans="2:10" ht="18">
-      <c r="B3" s="83"/>
+      <c r="B3" s="82"/>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="128" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="130"/>
+        <v>25</v>
+      </c>
+      <c r="C4" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="131"/>
     </row>
     <row r="5" spans="2:10" ht="18">
-      <c r="B5" s="83"/>
-    </row>
-    <row r="6" spans="2:10" s="84" customFormat="1" ht="34.5" customHeight="1">
+      <c r="B5" s="82"/>
+    </row>
+    <row r="6" spans="2:10" s="83" customFormat="1" ht="34.5" customHeight="1">
       <c r="B6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="128" customFormat="1">
       <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="C7" s="127" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="13">
         <v>42290</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="14">
+        <v>47</v>
+      </c>
+      <c r="F7" s="13">
         <v>42297</v>
       </c>
       <c r="G7" s="12">
         <v>4</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15">

</xml_diff>

<commit_message>
Registro de cambios de requerimientos
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_REQM/RCREQM/RCREQM_V1.1_2015.xlsx
+++ b/Area_de_Proceso-_REQM/RCREQM/RCREQM_V1.1_2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTP-GPS-ALARM\UTP-GPS-ALARM\Area_de_Proceso-_REQM\RCREQM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thefa\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_REQM\RCREQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="1" r:id="rId1"/>
@@ -65,12 +65,6 @@
     <t>Responsable de Revisión y/o Aprobación</t>
   </si>
   <si>
-    <t>Version Preliminar</t>
-  </si>
-  <si>
-    <t>En Revisión</t>
-  </si>
-  <si>
     <t>RCREQM Registro de Cambios de Requerimientos</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>Roger Apaéstegui</t>
   </si>
   <si>
-    <t>Version Preliminar aprobada por QA</t>
-  </si>
-  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -225,12 +216,21 @@
   </si>
   <si>
     <t>Versión: 1.1</t>
+  </si>
+  <si>
+    <t>Version Preliminar revisada por QA</t>
+  </si>
+  <si>
+    <t>Revisado</t>
+  </si>
+  <si>
+    <t>Version Final pendiente de Aprobación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -713,10 +713,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -725,89 +733,47 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -819,38 +785,72 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1447,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1456,7 +1456,7 @@
     <col min="1" max="3" width="9.140625" style="15" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="15" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="18" style="15" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="15" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="15" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="15" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="15"/>
@@ -1524,79 +1524,86 @@
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="14"/>
-      <c r="B5" s="84">
+      <c r="B5" s="86">
         <v>1</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="89">
+        <v>42290</v>
+      </c>
+      <c r="E5" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="86">
-        <v>42290</v>
-      </c>
-      <c r="E5" s="84" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="84" t="s">
-        <v>55</v>
+      <c r="F5" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="86" t="s">
+        <v>53</v>
       </c>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1">
       <c r="A6" s="14"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="14"/>
-      <c r="B7" s="84">
+      <c r="B7" s="86">
         <v>1</v>
       </c>
-      <c r="C7" s="85" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="86">
+      <c r="C7" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="89">
         <v>42313</v>
       </c>
-      <c r="E7" s="84" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="84" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="84" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="84" t="s">
-        <v>55</v>
+      <c r="E7" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="86" t="s">
+        <v>53</v>
       </c>
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="B8" s="84"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="10" spans="1:9" ht="48" customHeight="1"/>
     <row r="11" spans="1:9" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="B2:H2"/>
@@ -1605,13 +1612,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1639,24 +1639,24 @@
     <row r="2" spans="1:8" ht="48.75" customHeight="1">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="90" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92"/>
+      <c r="C2" s="118" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="120"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="17"/>
       <c r="B3" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="93" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="95"/>
+        <v>58</v>
+      </c>
+      <c r="C3" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="123"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="17"/>
@@ -1671,7 +1671,7 @@
     <row r="5" spans="1:8" ht="13.5">
       <c r="A5" s="17"/>
       <c r="B5" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="17"/>
       <c r="E5" s="25"/>
@@ -1680,13 +1680,13 @@
     </row>
     <row r="6" spans="1:8" ht="17.25" customHeight="1">
       <c r="A6" s="17"/>
-      <c r="B6" s="96" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="98"/>
+      <c r="B6" s="124" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="126"/>
     </row>
     <row r="7" spans="1:8" s="28" customFormat="1" ht="16.5" customHeight="1">
       <c r="A7" s="17"/>
@@ -1710,15 +1710,15 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="17"/>
-      <c r="B9" s="99" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="99"/>
+      <c r="B9" s="127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="127"/>
       <c r="D9" s="29"/>
-      <c r="E9" s="99" t="s">
+      <c r="E9" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="99"/>
+      <c r="F9" s="127"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17"/>
@@ -1728,14 +1728,14 @@
     </row>
     <row r="11" spans="1:8" ht="12" customHeight="1">
       <c r="A11" s="17"/>
-      <c r="B11" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="88"/>
-      <c r="E11" s="89" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="89"/>
+      <c r="B11" s="117" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="117"/>
+      <c r="E11" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="114"/>
     </row>
     <row r="12" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="17"/>
@@ -1744,42 +1744,42 @@
     </row>
     <row r="13" spans="1:8" ht="12" customHeight="1">
       <c r="A13" s="17"/>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="113"/>
+      <c r="E13" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="103"/>
-      <c r="E13" s="89" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="89"/>
+      <c r="F13" s="114"/>
     </row>
     <row r="14" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="12" customHeight="1">
       <c r="A15" s="32"/>
-      <c r="B15" s="104" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="104"/>
-      <c r="E15" s="89" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="89"/>
+      <c r="B15" s="115" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="115"/>
+      <c r="E15" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="114"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="32"/>
     </row>
     <row r="17" spans="1:9" ht="12" customHeight="1">
       <c r="A17" s="32"/>
-      <c r="B17" s="105" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="105"/>
-      <c r="E17" s="89" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="89"/>
+      <c r="B17" s="116" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="116"/>
+      <c r="E17" s="114" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="114"/>
       <c r="I17" s="33"/>
     </row>
     <row r="18" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1">
@@ -1794,46 +1794,46 @@
       <c r="A19" s="32"/>
     </row>
     <row r="20" spans="1:9" s="36" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="107" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
+    </row>
+    <row r="21" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B21" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="109"/>
+      <c r="D21" s="110" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="110"/>
+      <c r="F21" s="110"/>
+    </row>
+    <row r="22" spans="1:9" s="36" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B22" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="106"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106"/>
-    </row>
-    <row r="21" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B21" s="107" t="s">
+      <c r="C22" s="103"/>
+      <c r="D22" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="108"/>
-      <c r="D21" s="109" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-    </row>
-    <row r="22" spans="1:9" s="36" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B22" s="100" t="s">
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+    </row>
+    <row r="23" spans="1:9" s="36" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B23" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="102" t="s">
+      <c r="C23" s="103"/>
+      <c r="D23" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-    </row>
-    <row r="23" spans="1:9" s="36" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B23" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="101"/>
-      <c r="D23" s="102" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="101"/>
     </row>
     <row r="24" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
       <c r="B24" s="5"/>
@@ -1848,162 +1848,162 @@
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:9" s="36" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B26" s="106" t="s">
+      <c r="B26" s="107" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="107"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
+    </row>
+    <row r="27" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B27" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="109"/>
+      <c r="D27" s="110" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+    </row>
+    <row r="28" spans="1:9" s="36" customFormat="1">
+      <c r="B28" s="111" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="111"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="112"/>
+    </row>
+    <row r="29" spans="1:9" s="36" customFormat="1">
+      <c r="B29" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="106"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106"/>
-    </row>
-    <row r="27" spans="1:9" s="36" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B27" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="108"/>
-      <c r="D27" s="109" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-    </row>
-    <row r="28" spans="1:9" s="36" customFormat="1">
-      <c r="B28" s="112" t="s">
+      <c r="C29" s="100"/>
+      <c r="D29" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="112"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="113"/>
-    </row>
-    <row r="29" spans="1:9" s="36" customFormat="1">
-      <c r="B29" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="111"/>
-      <c r="D29" s="102" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="102"/>
-      <c r="F29" s="102"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="32"/>
-      <c r="B30" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="112"/>
-      <c r="D30" s="113"/>
-      <c r="E30" s="113"/>
-      <c r="F30" s="113"/>
+      <c r="B30" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="111"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="112"/>
     </row>
     <row r="31" spans="1:9" s="38" customFormat="1">
       <c r="A31" s="37"/>
-      <c r="B31" s="110" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="111"/>
-      <c r="D31" s="102" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="102"/>
-      <c r="F31" s="102"/>
+      <c r="B31" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="100"/>
+      <c r="D31" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
     </row>
     <row r="32" spans="1:9" s="38" customFormat="1">
       <c r="A32" s="37"/>
-      <c r="B32" s="110" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="111"/>
-      <c r="D32" s="102" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="102"/>
-      <c r="F32" s="102"/>
+      <c r="B32" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="100"/>
+      <c r="D32" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
     </row>
     <row r="33" spans="1:9" s="38" customFormat="1">
       <c r="A33" s="37"/>
-      <c r="B33" s="110" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="111"/>
-      <c r="D33" s="102" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="102"/>
-      <c r="F33" s="102"/>
+      <c r="B33" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="100"/>
+      <c r="D33" s="101" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
     </row>
     <row r="34" spans="1:9" s="38" customFormat="1">
       <c r="A34" s="37"/>
-      <c r="B34" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="111"/>
-      <c r="D34" s="102" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="102"/>
-      <c r="F34" s="102"/>
+      <c r="B34" s="99" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="100"/>
+      <c r="D34" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
     </row>
     <row r="35" spans="1:9" s="38" customFormat="1">
       <c r="A35" s="37"/>
-      <c r="B35" s="110" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="111"/>
-      <c r="D35" s="102" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="102"/>
-      <c r="F35" s="102"/>
+      <c r="B35" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="100"/>
+      <c r="D35" s="101" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="101"/>
+      <c r="F35" s="101"/>
     </row>
     <row r="36" spans="1:9" s="38" customFormat="1">
       <c r="A36" s="37"/>
-      <c r="B36" s="110" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="111"/>
-      <c r="D36" s="102" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="102"/>
-      <c r="F36" s="102"/>
+      <c r="B36" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="100"/>
+      <c r="D36" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="101"/>
+      <c r="F36" s="101"/>
     </row>
     <row r="37" spans="1:9" s="38" customFormat="1">
       <c r="A37" s="37"/>
-      <c r="B37" s="110" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="111"/>
-      <c r="D37" s="102" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="102"/>
-      <c r="F37" s="102"/>
+      <c r="B37" s="99" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="100"/>
+      <c r="D37" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="101"/>
+      <c r="F37" s="101"/>
     </row>
     <row r="38" spans="1:9" s="38" customFormat="1">
       <c r="A38" s="37"/>
-      <c r="B38" s="100" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="102" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="102"/>
-      <c r="F38" s="102"/>
+      <c r="B38" s="102" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="103"/>
+      <c r="D38" s="101" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="101"/>
+      <c r="F38" s="101"/>
     </row>
     <row r="39" spans="1:9" s="38" customFormat="1">
       <c r="A39" s="37"/>
-      <c r="B39" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="102" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="102"/>
-      <c r="F39" s="102"/>
+      <c r="B39" s="102" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="103"/>
+      <c r="D39" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
     </row>
     <row r="40" spans="1:9" ht="26.25" customHeight="1">
       <c r="A40" s="32"/>
@@ -2020,13 +2020,13 @@
     </row>
     <row r="42" spans="1:9" hidden="1">
       <c r="A42" s="32"/>
-      <c r="B42" s="115" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="115"/>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
-      <c r="F42" s="116"/>
+      <c r="B42" s="104" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="104"/>
+      <c r="D42" s="105"/>
+      <c r="E42" s="105"/>
+      <c r="F42" s="105"/>
       <c r="G42" s="41"/>
       <c r="H42" s="41"/>
       <c r="I42" s="41"/>
@@ -2044,7 +2044,7 @@
         <v>4</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G43" s="41"/>
       <c r="H43" s="41"/>
@@ -2118,9 +2118,9 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="34"/>
-      <c r="B50" s="117"/>
-      <c r="C50" s="117"/>
-      <c r="D50" s="117"/>
+      <c r="B50" s="106"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="106"/>
       <c r="E50" s="49"/>
       <c r="F50" s="48"/>
       <c r="G50" s="41"/>
@@ -2129,9 +2129,9 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="34"/>
-      <c r="B51" s="117"/>
-      <c r="C51" s="117"/>
-      <c r="D51" s="117"/>
+      <c r="B51" s="106"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="106"/>
       <c r="E51" s="50"/>
       <c r="F51" s="48"/>
       <c r="G51" s="41"/>
@@ -2206,9 +2206,9 @@
     </row>
     <row r="58" spans="1:9" ht="20.25" customHeight="1">
       <c r="A58" s="34"/>
-      <c r="B58" s="114"/>
-      <c r="C58" s="114"/>
-      <c r="D58" s="114"/>
+      <c r="B58" s="97"/>
+      <c r="C58" s="97"/>
+      <c r="D58" s="97"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="41"/>
@@ -2239,9 +2239,9 @@
     </row>
     <row r="61" spans="1:9" ht="30.75" customHeight="1">
       <c r="A61" s="34"/>
-      <c r="B61" s="114"/>
-      <c r="C61" s="114"/>
-      <c r="D61" s="114"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="97"/>
       <c r="E61" s="53"/>
       <c r="F61" s="3"/>
       <c r="G61" s="41"/>
@@ -2294,9 +2294,9 @@
     </row>
     <row r="66" spans="1:9" ht="27.75" customHeight="1">
       <c r="A66" s="34"/>
-      <c r="B66" s="114"/>
-      <c r="C66" s="114"/>
-      <c r="D66" s="114"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="97"/>
+      <c r="D66" s="97"/>
       <c r="E66" s="53"/>
       <c r="F66" s="3"/>
       <c r="G66" s="41"/>
@@ -2368,9 +2368,9 @@
     </row>
     <row r="73" spans="1:9" ht="17.25" customHeight="1">
       <c r="A73" s="34"/>
-      <c r="B73" s="114"/>
-      <c r="C73" s="114"/>
-      <c r="D73" s="114"/>
+      <c r="B73" s="97"/>
+      <c r="C73" s="97"/>
+      <c r="D73" s="97"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="41"/>
@@ -2379,9 +2379,9 @@
     </row>
     <row r="74" spans="1:9" ht="17.25" customHeight="1">
       <c r="A74" s="34"/>
-      <c r="B74" s="114"/>
-      <c r="C74" s="114"/>
-      <c r="D74" s="114"/>
+      <c r="B74" s="97"/>
+      <c r="C74" s="97"/>
+      <c r="D74" s="97"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="41"/>
@@ -2390,9 +2390,9 @@
     </row>
     <row r="75" spans="1:9" ht="17.25" customHeight="1">
       <c r="A75" s="34"/>
-      <c r="B75" s="114"/>
-      <c r="C75" s="114"/>
-      <c r="D75" s="114"/>
+      <c r="B75" s="97"/>
+      <c r="C75" s="97"/>
+      <c r="D75" s="97"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="41"/>
@@ -2401,9 +2401,9 @@
     </row>
     <row r="76" spans="1:9" ht="23.25" customHeight="1">
       <c r="A76" s="34"/>
-      <c r="B76" s="114"/>
-      <c r="C76" s="114"/>
-      <c r="D76" s="114"/>
+      <c r="B76" s="97"/>
+      <c r="C76" s="97"/>
+      <c r="D76" s="97"/>
       <c r="E76" s="53"/>
       <c r="F76" s="3"/>
       <c r="G76" s="41"/>
@@ -2677,8 +2677,8 @@
       <c r="B101" s="62"/>
       <c r="C101" s="62"/>
       <c r="D101" s="3"/>
-      <c r="E101" s="120"/>
-      <c r="F101" s="120"/>
+      <c r="E101" s="96"/>
+      <c r="F101" s="96"/>
       <c r="G101" s="41"/>
       <c r="H101" s="41"/>
       <c r="I101" s="41"/>
@@ -2978,11 +2978,11 @@
     </row>
     <row r="130" spans="1:6" ht="30.75" customHeight="1">
       <c r="A130" s="3"/>
-      <c r="B130" s="121"/>
-      <c r="C130" s="121"/>
-      <c r="D130" s="121"/>
-      <c r="E130" s="121"/>
-      <c r="F130" s="121"/>
+      <c r="B130" s="98"/>
+      <c r="C130" s="98"/>
+      <c r="D130" s="98"/>
+      <c r="E130" s="98"/>
+      <c r="F130" s="98"/>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="3"/>
@@ -2996,9 +2996,9 @@
       <c r="A132" s="3"/>
       <c r="B132" s="71"/>
       <c r="C132" s="71"/>
-      <c r="D132" s="119"/>
-      <c r="E132" s="119"/>
-      <c r="F132" s="119"/>
+      <c r="D132" s="92"/>
+      <c r="E132" s="92"/>
+      <c r="F132" s="92"/>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" s="3"/>
@@ -3012,9 +3012,9 @@
       <c r="A134" s="3"/>
       <c r="B134" s="73"/>
       <c r="C134" s="73"/>
-      <c r="D134" s="118"/>
-      <c r="E134" s="119"/>
-      <c r="F134" s="119"/>
+      <c r="D134" s="94"/>
+      <c r="E134" s="92"/>
+      <c r="F134" s="92"/>
     </row>
     <row r="135" spans="1:6">
       <c r="A135" s="3"/>
@@ -3028,9 +3028,9 @@
       <c r="A136" s="3"/>
       <c r="B136" s="71"/>
       <c r="C136" s="71"/>
-      <c r="D136" s="119"/>
-      <c r="E136" s="119"/>
-      <c r="F136" s="119"/>
+      <c r="D136" s="92"/>
+      <c r="E136" s="92"/>
+      <c r="F136" s="92"/>
     </row>
     <row r="137" spans="1:6">
       <c r="A137" s="3"/>
@@ -3044,9 +3044,9 @@
       <c r="A138" s="3"/>
       <c r="B138" s="73"/>
       <c r="C138" s="73"/>
-      <c r="D138" s="118"/>
-      <c r="E138" s="119"/>
-      <c r="F138" s="119"/>
+      <c r="D138" s="94"/>
+      <c r="E138" s="92"/>
+      <c r="F138" s="92"/>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="3"/>
@@ -3068,9 +3068,9 @@
       <c r="A141" s="3"/>
       <c r="B141" s="71"/>
       <c r="C141" s="71"/>
-      <c r="D141" s="119"/>
-      <c r="E141" s="119"/>
-      <c r="F141" s="119"/>
+      <c r="D141" s="92"/>
+      <c r="E141" s="92"/>
+      <c r="F141" s="92"/>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="3"/>
@@ -3084,113 +3084,113 @@
       <c r="A143" s="3"/>
       <c r="B143" s="73"/>
       <c r="C143" s="73"/>
-      <c r="D143" s="118"/>
-      <c r="E143" s="119"/>
-      <c r="F143" s="119"/>
+      <c r="D143" s="94"/>
+      <c r="E143" s="92"/>
+      <c r="F143" s="92"/>
     </row>
     <row r="144" spans="1:6" ht="90" customHeight="1">
       <c r="A144" s="3"/>
       <c r="B144" s="73"/>
       <c r="C144" s="73"/>
-      <c r="D144" s="118"/>
-      <c r="E144" s="119"/>
-      <c r="F144" s="119"/>
+      <c r="D144" s="94"/>
+      <c r="E144" s="92"/>
+      <c r="F144" s="92"/>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="3"/>
       <c r="B145" s="73"/>
       <c r="C145" s="73"/>
-      <c r="D145" s="123"/>
-      <c r="E145" s="120"/>
-      <c r="F145" s="120"/>
+      <c r="D145" s="95"/>
+      <c r="E145" s="96"/>
+      <c r="F145" s="96"/>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="3"/>
       <c r="B146" s="75"/>
       <c r="C146" s="75"/>
-      <c r="D146" s="122"/>
-      <c r="E146" s="122"/>
+      <c r="D146" s="91"/>
+      <c r="E146" s="91"/>
       <c r="F146" s="76"/>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" s="3"/>
       <c r="B147" s="75"/>
       <c r="C147" s="75"/>
-      <c r="D147" s="122"/>
-      <c r="E147" s="122"/>
+      <c r="D147" s="91"/>
+      <c r="E147" s="91"/>
       <c r="F147" s="76"/>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="3"/>
       <c r="B148" s="75"/>
       <c r="C148" s="75"/>
-      <c r="D148" s="122"/>
-      <c r="E148" s="122"/>
+      <c r="D148" s="91"/>
+      <c r="E148" s="91"/>
       <c r="F148" s="76"/>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="3"/>
       <c r="B149" s="75"/>
       <c r="C149" s="75"/>
-      <c r="D149" s="122"/>
-      <c r="E149" s="122"/>
+      <c r="D149" s="91"/>
+      <c r="E149" s="91"/>
       <c r="F149" s="76"/>
     </row>
     <row r="150" spans="1:6">
       <c r="A150" s="3"/>
       <c r="B150" s="75"/>
       <c r="C150" s="75"/>
-      <c r="D150" s="122"/>
-      <c r="E150" s="122"/>
+      <c r="D150" s="91"/>
+      <c r="E150" s="91"/>
       <c r="F150" s="76"/>
     </row>
     <row r="151" spans="1:6">
       <c r="A151" s="3"/>
       <c r="B151" s="75"/>
       <c r="C151" s="75"/>
-      <c r="D151" s="122"/>
-      <c r="E151" s="122"/>
+      <c r="D151" s="91"/>
+      <c r="E151" s="91"/>
       <c r="F151" s="76"/>
     </row>
     <row r="152" spans="1:6">
       <c r="A152" s="3"/>
       <c r="B152" s="75"/>
       <c r="C152" s="75"/>
-      <c r="D152" s="122"/>
-      <c r="E152" s="122"/>
+      <c r="D152" s="91"/>
+      <c r="E152" s="91"/>
       <c r="F152" s="77"/>
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="3"/>
       <c r="B153" s="75"/>
       <c r="C153" s="75"/>
-      <c r="D153" s="122"/>
-      <c r="E153" s="122"/>
+      <c r="D153" s="91"/>
+      <c r="E153" s="91"/>
       <c r="F153" s="77"/>
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="3"/>
       <c r="B154" s="75"/>
       <c r="C154" s="75"/>
-      <c r="D154" s="122"/>
-      <c r="E154" s="122"/>
+      <c r="D154" s="91"/>
+      <c r="E154" s="91"/>
       <c r="F154" s="77"/>
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="3"/>
       <c r="B155" s="75"/>
       <c r="C155" s="75"/>
-      <c r="D155" s="122"/>
-      <c r="E155" s="122"/>
+      <c r="D155" s="91"/>
+      <c r="E155" s="91"/>
       <c r="F155" s="77"/>
     </row>
     <row r="156" spans="1:6" ht="26.25" customHeight="1">
       <c r="A156" s="3"/>
       <c r="B156" s="75"/>
       <c r="C156" s="75"/>
-      <c r="D156" s="124"/>
-      <c r="E156" s="124"/>
-      <c r="F156" s="124"/>
+      <c r="D156" s="93"/>
+      <c r="E156" s="93"/>
+      <c r="F156" s="93"/>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="3"/>
@@ -3242,97 +3242,97 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="3"/>
-      <c r="B163" s="122"/>
-      <c r="C163" s="122"/>
-      <c r="D163" s="122"/>
+      <c r="B163" s="91"/>
+      <c r="C163" s="91"/>
+      <c r="D163" s="91"/>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="3"/>
-      <c r="B164" s="122"/>
-      <c r="C164" s="122"/>
-      <c r="D164" s="122"/>
+      <c r="B164" s="91"/>
+      <c r="C164" s="91"/>
+      <c r="D164" s="91"/>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="3"/>
-      <c r="B165" s="122"/>
-      <c r="C165" s="122"/>
-      <c r="D165" s="122"/>
+      <c r="B165" s="91"/>
+      <c r="C165" s="91"/>
+      <c r="D165" s="91"/>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="3"/>
-      <c r="B166" s="122"/>
-      <c r="C166" s="122"/>
-      <c r="D166" s="122"/>
+      <c r="B166" s="91"/>
+      <c r="C166" s="91"/>
+      <c r="D166" s="91"/>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="3"/>
-      <c r="B167" s="122"/>
-      <c r="C167" s="122"/>
-      <c r="D167" s="122"/>
+      <c r="B167" s="91"/>
+      <c r="C167" s="91"/>
+      <c r="D167" s="91"/>
       <c r="E167" s="3"/>
       <c r="F167" s="3"/>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="3"/>
-      <c r="B168" s="122"/>
-      <c r="C168" s="122"/>
-      <c r="D168" s="122"/>
+      <c r="B168" s="91"/>
+      <c r="C168" s="91"/>
+      <c r="D168" s="91"/>
       <c r="E168" s="3"/>
       <c r="F168" s="3"/>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="3"/>
-      <c r="B169" s="122"/>
-      <c r="C169" s="122"/>
-      <c r="D169" s="122"/>
+      <c r="B169" s="91"/>
+      <c r="C169" s="91"/>
+      <c r="D169" s="91"/>
       <c r="E169" s="3"/>
       <c r="F169" s="3"/>
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="3"/>
-      <c r="B170" s="122"/>
-      <c r="C170" s="122"/>
-      <c r="D170" s="122"/>
+      <c r="B170" s="91"/>
+      <c r="C170" s="91"/>
+      <c r="D170" s="91"/>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="3"/>
-      <c r="B171" s="122"/>
-      <c r="C171" s="122"/>
-      <c r="D171" s="122"/>
+      <c r="B171" s="91"/>
+      <c r="C171" s="91"/>
+      <c r="D171" s="91"/>
       <c r="E171" s="3"/>
       <c r="F171" s="3"/>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="3"/>
-      <c r="B172" s="122"/>
-      <c r="C172" s="122"/>
-      <c r="D172" s="122"/>
+      <c r="B172" s="91"/>
+      <c r="C172" s="91"/>
+      <c r="D172" s="91"/>
       <c r="E172" s="3"/>
       <c r="F172" s="3"/>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="3"/>
-      <c r="B173" s="122"/>
-      <c r="C173" s="122"/>
-      <c r="D173" s="122"/>
+      <c r="B173" s="91"/>
+      <c r="C173" s="91"/>
+      <c r="D173" s="91"/>
       <c r="E173" s="3"/>
       <c r="F173" s="3"/>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="3"/>
-      <c r="B174" s="122"/>
-      <c r="C174" s="122"/>
-      <c r="D174" s="122"/>
+      <c r="B174" s="91"/>
+      <c r="C174" s="91"/>
+      <c r="D174" s="91"/>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
     </row>
@@ -3346,19 +3346,19 @@
     </row>
     <row r="176" spans="1:6" ht="15" customHeight="1">
       <c r="A176" s="73"/>
-      <c r="B176" s="119"/>
-      <c r="C176" s="119"/>
-      <c r="D176" s="119"/>
-      <c r="E176" s="119"/>
-      <c r="F176" s="119"/>
+      <c r="B176" s="92"/>
+      <c r="C176" s="92"/>
+      <c r="D176" s="92"/>
+      <c r="E176" s="92"/>
+      <c r="F176" s="92"/>
     </row>
     <row r="177" spans="1:6" ht="32.25" customHeight="1">
       <c r="A177" s="73"/>
-      <c r="B177" s="119"/>
-      <c r="C177" s="119"/>
-      <c r="D177" s="119"/>
-      <c r="E177" s="119"/>
-      <c r="F177" s="119"/>
+      <c r="B177" s="92"/>
+      <c r="C177" s="92"/>
+      <c r="D177" s="92"/>
+      <c r="E177" s="92"/>
+      <c r="F177" s="92"/>
     </row>
     <row r="178" spans="1:6">
       <c r="A178" s="3"/>
@@ -3386,99 +3386,58 @@
     </row>
     <row r="181" spans="1:6" ht="32.25" customHeight="1">
       <c r="A181" s="73"/>
-      <c r="B181" s="125"/>
-      <c r="C181" s="125"/>
-      <c r="D181" s="125"/>
-      <c r="E181" s="125"/>
-      <c r="F181" s="125"/>
+      <c r="B181" s="90"/>
+      <c r="C181" s="90"/>
+      <c r="D181" s="90"/>
+      <c r="E181" s="90"/>
+      <c r="F181" s="90"/>
     </row>
     <row r="182" spans="1:6" ht="17.25" customHeight="1">
       <c r="A182" s="73"/>
-      <c r="B182" s="125"/>
-      <c r="C182" s="125"/>
-      <c r="D182" s="125"/>
-      <c r="E182" s="125"/>
-      <c r="F182" s="125"/>
+      <c r="B182" s="90"/>
+      <c r="C182" s="90"/>
+      <c r="D182" s="90"/>
+      <c r="E182" s="90"/>
+      <c r="F182" s="90"/>
     </row>
     <row r="183" spans="1:6" ht="18" customHeight="1">
       <c r="A183" s="73"/>
-      <c r="B183" s="125"/>
-      <c r="C183" s="125"/>
-      <c r="D183" s="125"/>
-      <c r="E183" s="125"/>
-      <c r="F183" s="125"/>
+      <c r="B183" s="90"/>
+      <c r="C183" s="90"/>
+      <c r="D183" s="90"/>
+      <c r="E183" s="90"/>
+      <c r="F183" s="90"/>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="73"/>
-      <c r="B184" s="125"/>
-      <c r="C184" s="125"/>
-      <c r="D184" s="125"/>
-      <c r="E184" s="125"/>
-      <c r="F184" s="125"/>
+      <c r="B184" s="90"/>
+      <c r="C184" s="90"/>
+      <c r="D184" s="90"/>
+      <c r="E184" s="90"/>
+      <c r="F184" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B174:D174"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B173:D173"/>
-    <mergeCell ref="D156:F156"/>
-    <mergeCell ref="B163:D163"/>
-    <mergeCell ref="B164:D164"/>
-    <mergeCell ref="B165:D165"/>
-    <mergeCell ref="B166:D166"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="B168:D168"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="B171:D171"/>
-    <mergeCell ref="B172:D172"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D144:F144"/>
-    <mergeCell ref="D145:F145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="D132:F132"/>
-    <mergeCell ref="D134:F134"/>
-    <mergeCell ref="D136:F136"/>
-    <mergeCell ref="D138:F138"/>
-    <mergeCell ref="D141:F141"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:F33"/>
     <mergeCell ref="B26:F26"/>
@@ -3492,26 +3451,67 @@
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:F32"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="D132:F132"/>
+    <mergeCell ref="D134:F134"/>
+    <mergeCell ref="D136:F136"/>
+    <mergeCell ref="D138:F138"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D144:F144"/>
+    <mergeCell ref="D145:F145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="B173:D173"/>
+    <mergeCell ref="D156:F156"/>
+    <mergeCell ref="B163:D163"/>
+    <mergeCell ref="B164:D164"/>
+    <mergeCell ref="B165:D165"/>
+    <mergeCell ref="B166:D166"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="B168:D168"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="B171:D171"/>
+    <mergeCell ref="B172:D172"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B174:D174"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
   </mergeCells>
   <conditionalFormatting sqref="B69:C70">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
@@ -3535,7 +3535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:J2"/>
     </sheetView>
   </sheetViews>
@@ -3556,26 +3556,26 @@
   <sheetData>
     <row r="2" spans="2:10" ht="48" customHeight="1">
       <c r="B2" s="80"/>
-      <c r="C2" s="126" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
+      <c r="C2" s="128" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
     </row>
     <row r="3" spans="2:10" ht="18">
       <c r="B3" s="82"/>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="129" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" s="130"/>
       <c r="E4" s="130"/>
@@ -3590,45 +3590,45 @@
     </row>
     <row r="6" spans="2:10" s="83" customFormat="1" ht="34.5" customHeight="1">
       <c r="B6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" s="128" customFormat="1">
+    </row>
+    <row r="7" spans="2:10" s="85" customFormat="1">
       <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="127" t="s">
-        <v>46</v>
+      <c r="C7" s="84" t="s">
+        <v>44</v>
       </c>
       <c r="D7" s="13">
         <v>42290</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F7" s="13">
         <v>42297</v>
@@ -3637,13 +3637,13 @@
         <v>4</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15">

</xml_diff>